<commit_message>
created testSimple table for sample project Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Sample Project/Main.xlsx
+++ b/DESIGN/rules/Sample Project/Main.xlsx
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Rule</t>
   </si>
@@ -258,13 +258,29 @@
   </si>
   <si>
     <t>Rules String Hello (Integer hour)</t>
+  </si>
+  <si>
+    <t>SimpleRules String TestSimple(String param1)</t>
+  </si>
+  <si>
+    <t>param1</t>
+  </si>
+  <si>
+    <t>RETURN</t>
+  </si>
+  <si>
+    <t>step1</t>
+  </si>
+  <si>
+    <t>run</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -306,8 +322,40 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color rgb="000001"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -338,8 +386,48 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="A6A6A6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="A6A6A6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAD246"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAD246"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="D9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="D9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -560,11 +648,395 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <top>
+        <color rgb="000000"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000000"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000000"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000000"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000000"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000000"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <bottom style="thick">
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thick">
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <top>
+        <color rgb="000001"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000001"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000001"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000001"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="000001"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="000001"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="000001"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000001"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -597,6 +1069,22 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="23" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="29" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="37" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="43" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="51" xfId="0" applyFill="true" applyBorder="true" applyAlignment="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -959,24 +1447,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E11"/>
+  <dimension ref="B3:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="2.85546875"/>
+    <col min="2" max="2" customWidth="true" style="1" width="5.42578125"/>
+    <col min="3" max="3" customWidth="true" style="1" width="18.7109375"/>
+    <col min="4" max="4" customWidth="true" style="1" width="19.0"/>
+    <col min="5" max="5" customWidth="true" style="1" width="24.28515625"/>
+    <col min="6" max="6" customWidth="true" style="1" width="25.85546875"/>
+    <col min="7" max="7" customWidth="true" style="1" width="11.42578125"/>
+    <col min="8" max="8" customWidth="true" style="1" width="12.85546875"/>
+    <col min="9" max="9" customWidth="true" style="1" width="14.28515625"/>
+    <col min="10" max="10" customWidth="true" style="1" width="12.85546875"/>
+    <col min="11" max="11" customWidth="true" style="1" width="13.0"/>
+    <col min="12" max="16384" style="1" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1095,9 +1583,32 @@
         <v>16</v>
       </c>
     </row>
+    <row r="13">
+      <c r="B13" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="32"/>
+    </row>
+    <row r="14">
+      <c r="B14" t="s" s="28">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s" s="29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s" s="30">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s" s="31">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
editing table Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Sample Project/Main.xlsx
+++ b/DESIGN/rules/Sample Project/Main.xlsx
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Rule</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>run</t>
+  </si>
+  <si>
+    <t>Good Morning2345</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1037,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1538,7 +1541,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
adding the field in testSimple table Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Sample Project/Main.xlsx
+++ b/DESIGN/rules/Sample Project/Main.xlsx
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Rule</t>
   </si>
@@ -276,6 +276,12 @@
   </si>
   <si>
     <t>Good Morning2345</t>
+  </si>
+  <si>
+    <t>step2</t>
+  </si>
+  <si>
+    <t>run2</t>
   </si>
 </sst>
 </file>
@@ -1450,7 +1456,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E15"/>
+  <dimension ref="B3:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
@@ -1608,6 +1614,14 @@
         <v>26</v>
       </c>
     </row>
+    <row r="16">
+      <c r="B16" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:E3"/>

</xml_diff>